<commit_message>
Build 2.0.0.6 - Added Include all versions for DqlDataSource Fixed Error Messaging grid. Fixed bug grid mapping not deleting correct item
</commit_message>
<xml_diff>
--- a/Fme.Library.Tests/dm_document1.xlsx
+++ b/Fme.Library.Tests/dm_document1.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jose17354\Documents\Verification tool\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="9885"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="9885" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="108">
   <si>
     <t>r_object_id</t>
   </si>
@@ -342,6 +338,12 @@
   </si>
   <si>
     <t>0602a0648000021b</t>
+  </si>
+  <si>
+    <t>a1|a3|a2</t>
+  </si>
+  <si>
+    <t>k1|k3|k2</t>
   </si>
 </sst>
 </file>
@@ -653,7 +655,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -663,16 +665,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CI11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.42578125" style="1" customWidth="1"/>
     <col min="2" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="27.28515625" customWidth="1"/>
     <col min="12" max="12" width="9.140625" style="1"/>
     <col min="18" max="18" width="9.140625" style="1"/>
+    <col min="20" max="20" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="25" width="9.140625" style="1"/>
     <col min="29" max="29" width="9.140625" style="1"/>
     <col min="32" max="32" width="9.140625" style="1"/>
@@ -972,10 +976,10 @@
         <v>90</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>90</v>
@@ -984,7 +988,7 @@
         <v>90</v>
       </c>
       <c r="J2" s="2">
-        <v>41556.377268518518</v>
+        <v>41556.252268518518</v>
       </c>
       <c r="K2" s="2">
         <v>41556.377268518518</v>
@@ -1014,7 +1018,7 @@
         <v>0</v>
       </c>
       <c r="T2">
-        <v>1</v>
+        <v>1.01</v>
       </c>
       <c r="U2">
         <v>1</v>
@@ -1235,10 +1239,10 @@
         <v>90</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>90</v>
@@ -1247,7 +1251,7 @@
         <v>90</v>
       </c>
       <c r="J3" s="2">
-        <v>41556.377268518518</v>
+        <v>41556.252268518518</v>
       </c>
       <c r="K3" s="2">
         <v>41556.377268518518</v>
@@ -1852,4 +1856,48 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>